<commit_message>
update hardware pe area and power sheet
</commit_message>
<xml_diff>
--- a/hardware/PE_Area_Power.xlsx
+++ b/hardware/PE_Area_Power.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chenyuzong/Desktop/BitMoD/hardware/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C08C85B-BD49-4B49-ADC5-319B6047F3FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E9A0E87-87A1-744B-8FE3-26F1FC099C3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26840" xr2:uid="{0EA28085-E4A3-684E-9F0D-9CE11563B083}"/>
   </bookViews>
@@ -78,6 +78,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -123,7 +126,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -443,7 +446,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="314" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -478,7 +481,7 @@
         <v>306.89999999999998</v>
       </c>
       <c r="D2" s="3">
-        <v>1.5299999999999999E-2</v>
+        <v>0.13600000000000001</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -492,7 +495,7 @@
         <v>748.3</v>
       </c>
       <c r="D3" s="3">
-        <v>2.4299999999999999E-2</v>
+        <v>0.185</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -505,8 +508,8 @@
       <c r="C4" s="1">
         <v>546.1</v>
       </c>
-      <c r="D4" s="1">
-        <v>0.15</v>
+      <c r="D4" s="3">
+        <v>0.19500000000000001</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -519,8 +522,8 @@
       <c r="C5" s="1">
         <v>192.4</v>
       </c>
-      <c r="D5" s="1">
-        <v>0.1</v>
+      <c r="D5" s="3">
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -534,6 +537,10 @@
       <c r="C6" s="2">
         <f>C2+C3+C4+C5</f>
         <v>1793.6999999999998</v>
+      </c>
+      <c r="D6" s="2">
+        <f>D2+D3+D4+D5</f>
+        <v>0.58600000000000008</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>